<commit_message>
adding a bunch of data and a lot of other changes for the last days
</commit_message>
<xml_diff>
--- a/data/Eksklusionslister/AP Pension_eksklusionsliste_isin.xlsx
+++ b/data/Eksklusionslister/AP Pension_eksklusionsliste_isin.xlsx
@@ -873,7 +873,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>['Fredericia', 'Greve', 'Herning', 'Hillerød', 'Høje Taastrup', 'Hørsholm', 'Kolding', 'Lemvig', 'Næstved', 'Randers', 'Skive', 'Varde', 'Aabenraa', 'Furesø', 'Ringkøbing-Skjern', 'Horsens', 'Mariagerfjord', 'Skanderborg', 'Syddjurs', 'Esbjerg', 'København', 'Odense', 'Aarhus']</t>
+          <t>['Fredericia', 'Greve', 'Herning', 'Hillerød', 'Høje Taastrup', 'Hørsholm', 'Kolding', 'Lemvig', 'Næstved', 'Randers', 'Skive', 'Varde', 'Aabenraa', 'Furesø', 'Ringkøbing-Skjern', 'Horsens', 'Mariagerfjord', 'Skanderborg', 'Syddjurs', 'København', 'Odense', 'Esbjerg', 'Aarhus']</t>
         </is>
       </c>
     </row>
@@ -4568,7 +4568,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>['4,5 ENAPCL 14-09-2047 (REGS)', 'EMPRESA NACIONAL DEL PET 5.25% 06.11.2029', '5,25 ENAPCL 06-11-2029 (REGS)']</t>
+          <t>['4,5 ENAPCL 14-09-2047 (REGS)', '5,25 ENAPCL 06-11-2029 (REGS)', 'EMPRESA NACIONAL DEL PET 5.25% 06.11.2029']</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>['6,7 PEMEX 16-02-2032', 'PETROLEOS MEXICANOS 6.75% 21.09.2047', '6,75 PEMEX 21-09-2047', '6,5 PEMEX 13-03-2027', '5,35 PEMEX 12-02-2028', 'PETROLEOS MEXICANOS 6.84% 23.01.2030', 'PETROLEOS MEXICANOS 7.69% 23.01.2050', 'PETROLEOS MEXICANOS 6.95% 28.01.2060', 'PETROLEOS MEXICANOS 7.19% 12.09.2024', 'PETROLEOS MEXICANOS 2.75% 21.04.2027', 'PETROLEOS MEXICANOS 4.75% 26.02.2029', 'PETROLEOS MEXICANOS 3.625% 24.11.2025']</t>
+          <t>['6,7 PEMEX 16-02-2032', '6,75 PEMEX 21-09-2047', 'PETROLEOS MEXICANOS 6.75% 21.09.2047', '6,5 PEMEX 13-03-2027', '5,35 PEMEX 12-02-2028', 'PETROLEOS MEXICANOS 6.84% 23.01.2030', 'PETROLEOS MEXICANOS 7.69% 23.01.2050', 'PETROLEOS MEXICANOS 6.95% 28.01.2060', 'PETROLEOS MEXICANOS 7.19% 12.09.2024', 'PETROLEOS MEXICANOS 2.75% 21.04.2027', 'PETROLEOS MEXICANOS 4.75% 26.02.2029', 'PETROLEOS MEXICANOS 3.625% 24.11.2025']</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
@@ -8781,17 +8781,17 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>['Qatar', 'QATAR ENERGY  ', 'QatarEnergy']</t>
+          <t>['QatarEnergy', 'Qatar', 'QATAR ENERGY  ']</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>['QATAR ENERGY 2.25% 12.07.2031', '2,25 QPETRO 12-07-2031 (REGS)']</t>
+          <t>['2,25 QPETRO 12-07-2031 (REGS)', 'QATAR ENERGY 2.25% 12.07.2031']</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>['Fanø', 'Kalundborg', 'Herning', 'Rødovre', 'Vejen']</t>
+          <t>['Herning', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen']</t>
         </is>
       </c>
     </row>
@@ -12666,17 +12666,17 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>['9.50% Angolan Government International Bond 2025', 'Angolan Government International Bond', '8.25% Angolan Government International Bond 2028', 'Angola', 'Republic of Angola', 'REPUBLIC OF ANGOLA  ', '8.75% Angolan Government International Bond 2032']</t>
+          <t>['9.50% Angolan Government International Bond 2025', 'Angolan Government International Bond', 'Republic of Angola', '8.25% Angolan Government International Bond 2028', 'Angola', 'REPUBLIC OF ANGOLA  ', '8.75% Angolan Government International Bond 2032']</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>['9.50% Angolan Government International Bond 2025', '8.25% Angolan Government International Bond 2028', 'REPUBLIC OF ANGOLA 8.25% 09.05.2028', '8,25 ANGOL 09-05-2028 (REGS)', 'REPUBLIC OF ANGOLA 9.375% 08.05.2048', 'REPUBLIC OF ANGOLA 8% 26.11.2029', 'REPUBLIC OF ANGOLA 9.125% 26.11.2049', '9,125 ANGOL 26-11-2049 (REGS)', '8.75% Angolan Government International Bond 2032', 'REPUBLIC OF ANGOLA 8.75% 14.04.2032', '8,75 ANGOL 14-04-2032 (REGS)']</t>
+          <t>['9.50% Angolan Government International Bond 2025', '8,25 ANGOL 09-05-2028 (REGS)', '8.25% Angolan Government International Bond 2028', 'REPUBLIC OF ANGOLA 8.25% 09.05.2028', 'REPUBLIC OF ANGOLA 9.375% 08.05.2048', 'REPUBLIC OF ANGOLA 8% 26.11.2029', '9,125 ANGOL 26-11-2049 (REGS)', 'REPUBLIC OF ANGOLA 9.125% 26.11.2049', '8,75 ANGOL 14-04-2032 (REGS)', '8.75% Angolan Government International Bond 2032', 'REPUBLIC OF ANGOLA 8.75% 14.04.2032']</t>
         </is>
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>['Ringkøbing-Skjern', 'Region Nordjylland', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen', 'Herning']</t>
+          <t>['Ringkøbing-Skjern', 'Region Nordjylland', 'Herning', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen']</t>
         </is>
       </c>
     </row>
@@ -12703,17 +12703,17 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>['Azerbaijan', 'Republic of Azerbaijan International Bond', 'Republic of Azerbaijan', 'REPUBLIC OF AZERBAIJAN  ']</t>
+          <t>['Azerbaijan', 'Republic of Azerbaijan', 'Republic of Azerbaijan International Bond', 'REPUBLIC OF AZERBAIJAN  ']</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>['SOUTHERN GAS CORRIDOR 6.875% 24.03.2026', 'REPUBLIC OF AZERBAIJAN 3.5% 01.09.2032', '3,5 AZERBJ 01-09-2032 (REGS)']</t>
+          <t>['SOUTHERN GAS CORRIDOR 6.875% 24.03.2026', '3,5 AZERBJ 01-09-2032 (REGS)', 'REPUBLIC OF AZERBAIJAN 3.5% 01.09.2032']</t>
         </is>
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>['Fanø', 'Kalundborg', 'Rødovre', 'Vejen', 'Herning']</t>
+          <t>['Fanø', 'Kalundborg', 'Herning', 'Rødovre', 'Vejen']</t>
         </is>
       </c>
     </row>
@@ -12782,7 +12782,7 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>['Commercial International Bank', 'Commercial International Bank - Egypt (CIB)', 'EFG Holding S.A.E.', 'ARAB REPUBLIC OF EGYPT 8.5% 31.01.2047', 'ARAB REPUBLIC OF EGYPT 7.903% 21.02.2048', 'ARAB REPUBLIC OF EGYPT 5.625% 16.04.2030', 'ARAB REPUBLIC OF EGYPT 7.6003% 01.03.2029', 'ARAB REPUBLIC OF EGYPT 4.75% 11.04.2025', 'ARAB REPUBLIC OF EGYPT 6.375% 11.04.2031', 'AFRICAN EXPORT-IMPORT BA 3.994% 21.09.2029', 'ARAB REPUBLIC OF EGYPT 7.0529% 15.01.2032', 'ARAB REPUBLIC OF EGYPT 8.875% 29.05.2050', 'ARAB REPUBLIC OF EGYPT 3.875% 16.02.2026', 'ARAB REPUBLIC OF EGYPT 7.5% 16.02.2061', 'AFRICAN EXPORT-IMPORT BA 3.798% 17.05.2031', 'EGYPT TASKEEK COMPANY 10.875% 28.02.2026', 'EGYPT TASKEEK CO 10.875% 28.02.2026']</t>
+          <t>['Commercial International Bank', 'Commercial International Bank - Egypt (CIB)', 'EFG Holding S.A.E.', 'ARAB REPUBLIC OF EGYPT 8.5% 31.01.2047', 'ARAB REPUBLIC OF EGYPT 7.903% 21.02.2048', 'ARAB REPUBLIC OF EGYPT 5.625% 16.04.2030', 'ARAB REPUBLIC OF EGYPT 7.6003% 01.03.2029', 'ARAB REPUBLIC OF EGYPT 4.75% 11.04.2025', 'ARAB REPUBLIC OF EGYPT 6.375% 11.04.2031', 'AFRICAN EXPORT-IMPORT BA 3.994% 21.09.2029', 'ARAB REPUBLIC OF EGYPT 7.0529% 15.01.2032', 'ARAB REPUBLIC OF EGYPT 8.875% 29.05.2050', 'ARAB REPUBLIC OF EGYPT 3.875% 16.02.2026', 'ARAB REPUBLIC OF EGYPT 7.5% 16.02.2061', 'AFRICAN EXPORT-IMPORT BA 3.798% 17.05.2031', 'EGYPT TASKEEK CO 10.875% 28.02.2026', 'EGYPT TASKEEK COMPANY 10.875% 28.02.2026']</t>
         </is>
       </c>
       <c r="G334" t="inlineStr">
@@ -12888,17 +12888,17 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>['Gabon Blue Bond Master Trust Series 2', nan, '6.10% Gabon Blue Bond Master Trust Series 2 2038', 'GABON BLUE BOND MASTER  ', 'USA', '6.95% Gabon Government International Bond 2025', 'Gabon', 'Gabon Government International Bond', 'REPUBLIC OF GABON  ']</t>
+          <t>['6.10% Gabon Blue Bond Master Trust Series 2 2038', 'Gabon Blue Bond Master Trust Series 2', 'GABON BLUE BOND MASTER  ', 'USA', nan, '6.95% Gabon Government International Bond 2025', 'Gabon Government International Bond', 'Gabon', 'REPUBLIC OF GABON  ']</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>['GABON BLUE BOND MASTER 6.097% 01.08.2038', 'Gabon Blue Bond Master Trust Series 2', '6.10% Gabon Blue Bond Master Trust Series 2 2038', '6.95% Gabon Government International Bond 2025', 'REPUBLIC OF GABON 6.95% 16.06.2025', 'REPUBLIC OF GABON 6.625% 06.02.2031', 'REPUBLIC OF GABON 7% 24.11.2031']</t>
+          <t>['6.10% Gabon Blue Bond Master Trust Series 2 2038', 'GABON BLUE BOND MASTER 6.097% 01.08.2038', 'Gabon Blue Bond Master Trust Series 2', '6.95% Gabon Government International Bond 2025', 'REPUBLIC OF GABON 6.95% 16.06.2025', 'REPUBLIC OF GABON 6.625% 06.02.2031', 'REPUBLIC OF GABON 7% 24.11.2031']</t>
         </is>
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>['Rødovre', 'Vejen', 'Svendborg', 'Ringkøbing-Skjern', 'Kalundborg', 'Region Nordjylland', 'Hedensted', 'Slagelse', 'Fanø']</t>
+          <t>['Ringkøbing-Skjern', 'Region Nordjylland', 'Rødovre', 'Vejen', 'Kalundborg', 'Fanø', 'Svendborg', 'Hedensted', 'Slagelse']</t>
         </is>
       </c>
     </row>
@@ -12962,17 +12962,17 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>['5.75% Jordan Government International Bond 2027', 'Jordan Government International Bond', nan, 'Hashemite Kingdom of Jordan', 'Jordan', 'KINGDOM OF JORDAN  ', '4.95% Jordan Government International Bond 2025', '7.75% Jordan Government International Bond 2028']</t>
+          <t>['5.75% Jordan Government International Bond 2027', 'Jordan Government International Bond', 'Hashemite Kingdom of Jordan', nan, 'Jordan', 'KINGDOM OF JORDAN  ', '4.95% Jordan Government International Bond 2025', '7.75% Jordan Government International Bond 2028']</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>['5.75% Jordan Government International Bond 2027', 'JORDAN 7 3/8 10/10/47', 'Jordan Government International Bond', '7,375 JORDAN 10-10-2047 (REGS)', 'KINGDOM OF JORDAN 7.375% 10.10.2047', 'KINGDOM OF JORDAN 5.85% 07.07.2030', '4.95% Jordan Government International Bond 2025', 'KINGDOM OF JORDAN 4.95% 07.07.2025', '7.75% Jordan Government International Bond 2028', '7,75 JORDAN 15-01-2028 (REGS)', 'KINGDOM OF JORDAN 7.5% 13.01.2029']</t>
+          <t>['5.75% Jordan Government International Bond 2027', '7,375 JORDAN 10-10-2047 (REGS)', 'JORDAN 7 3/8 10/10/47', 'Jordan Government International Bond', 'KINGDOM OF JORDAN 7.375% 10.10.2047', 'KINGDOM OF JORDAN 5.85% 07.07.2030', '4.95% Jordan Government International Bond 2025', 'KINGDOM OF JORDAN 4.95% 07.07.2025', '7,75 JORDAN 15-01-2028 (REGS)', '7.75% Jordan Government International Bond 2028', 'KINGDOM OF JORDAN 7.5% 13.01.2029']</t>
         </is>
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>['Ringkøbing-Skjern', 'Region Nordjylland', 'Guldborgsund', 'Nordfyn', 'Svendborg', 'Herning', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen', 'Hedensted', 'Slagelse']</t>
+          <t>['Ringkøbing-Skjern', 'Region Nordjylland', 'Herning', 'Guldborgsund', 'Nordfyn', 'Svendborg', 'Hedensted', 'Slagelse', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen']</t>
         </is>
       </c>
     </row>
@@ -13041,12 +13041,12 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>['CHINA GOVERNMENT BOND 2.67% 25.05.2033', 'Ping An Bank Co. Ltd.', 'CECEP Solar Energy Co. Ltd.', 'China Vanke Co. Ltd.', 'China Vanke Co Ltd', 'China Baoan Group Co. Ltd.', 'Fuyao Glass Industry Group Co.', 'Pangang Group Vanadium Titaniu', 'Sichuan Chuantou Energy Co. Ltd.', 'Shanghai Baosight Software Co.', 'XCMG Construction Machinery Co.', 'Inner Mongolia Yili Industrial', 'Inner Mongolia Yili Industrial Group Co Ltd', 'Wingtech Technology Co. Ltd.', 'Shanghai Jinjiang Internationa', 'Yutong Bus Co. Ltd.', 'AECC Aero-Engine Control Co. Lt', 'Yunnan Yuntianhua Co. Ltd.', 'Qinghai Salt Lake Industry Co. Ltd.', 'Shanghai International Airport', 'China CSSC Holdings Ltd.', 'Xiamen C &amp; D Inc.', 'Shanghai Construction Group Co.', 'Shanghai Fosun Pharmaceutical', 'Asia - Potash International Investment Guangzhou C', 'Unisplendour Corp. Ltd.', 'Jiangsu Eastern Shenghong Co. L', 'Shanghai International Port Gr', 'Jiangsu Hengrui Pharmaceutical', 'Jiangsu Hengrui Pharmaceuticals Co Ltd', 'Wanhua Chemical Group Co. Ltd.', 'China Avionics Systems Co Ltd A', 'China Merchants Bank Co. Ltd.', 'China Merchants Bank Co Ltd', 'Jiangsu Zhongtian Technology C', 'Jiangsu Zhongtian Technology', 'Jiangsu\xa0Zhongtian\xa0Technology', 'Xiamen Tungsten Co. Ltd.', 'CITIC Securities Co. Ltd.', 'Sichuan Road and Bridge Group', 'Zhangzhou Pientzehuang Pharmac', 'Zhangzhou Pientzehuang Pharmaceutical Co Ltd', 'Sany Heavy Industry Co. Ltd.', 'Zhongjin Gold Corp. Ltd.', 'NARI Technology Co. Ltd.', 'Tongwei Co. Ltd.', 'Zhejiang Sanhua Intelligent Controls Co. Ltd.', 'Bank of China Ltd.', 'Industrial &amp; Commercial Bank o', 'Industrial &amp; Commercial Bank of China Ltd', 'Sinoma Science &amp; Technology Co.', 'Industrial Bank Co. Ltd.', 'TCL Zhonghuan Renewable Energy', 'Bank of Ningbo Co. Ltd.', 'Western Mining Co. Ltd.', 'China Railway Group Ltd.', 'COSCO SHIPPING Development Co.', 'Goldwind Science &amp; Technology', 'Shanghai Electric Group Co. Ltd.', 'China State Construction Engin', 'Aier Eye Hospital Group Co. Ltd.', 'Eve Energy Co. Ltd.', 'Shenzhen Capchem Technology Co.', 'China National Chemical Engine', 'Zhejiang Chint Electrics Co. Lt', 'Zhejiang Chint Electrics Co Ltd', 'East Money Information Co. Ltd.', 'NAURA Technology Group Co. Ltd.', 'JA Solar Technology Co. Ltd.', 'Ganfeng Lithium Group Co. Ltd.', 'Ganfeng Lithium Group Co Ltd', 'Guangzhou Haige Communications', 'Shenzhen Inovance Technology C', 'Shenzhen Inovance Technology Co Ltd', 'Shenzhen Inovance Technology Co., Lt', 'Songcheng Performance Developm', 'Yonghui Superstores Co. Ltd.', 'Tianshan Aluminum Group Co. Ltd.', 'BYD Co. Ltd.', 'BYD Co Ltd', 'Sungrow Power Supply Co. Ltd.', 'Sungrow Power Supply Co Ltd', 'Kuang-Chi Technologies Co. Ltd.', 'Satellite Chemical Co. Ltd.', 'Zhongji Innolight Co. Ltd.', 'LONGi Green Energy Technology', 'Sichuan Hebang Biotechnology C', 'CMOC Group Ltd.', 'Guangzhou Tinci Materials Tech', 'Muyuan Foods Co. Ltd.', 'Foshan Haitian Flavouring &amp; Fo', 'Zhejiang Huayou Cobalt Co. Ltd.', 'Sinomine Resource Group Co. Ltd.', 'Orient Securities Co. Ltd/China', 'China National Nuclear Power C', 'Ningbo Tuopu Group Co. Ltd.', 'Wens Foodstuffs Group Co. Ltd.', 'Yealink Network Technology Cor', 'Foxconn Industrial Internet Co.', 'Contemporary Amperex Technolog', 'Contemporary Amperex Technology Co Ltd', 'Shenzhen Mindray Bio-Medical E', 'Shenzhen Mindray Bio-Medical Electronics Co Ltd', 'Shenzhen Transsion Holdings Co.', 'China Zheshang Bank Co. Ltd.', 'China Zheshang Bank Co Ltd', 'CNGR Advanced Material Co. Ltd.', 'Yunnan Botanee Bio-Technology Group Co. Ltd.', 'China Energy Engineering Corp.', 'China Three Gorges Renewables', 'China Three Gorges Renewables Group Co Ltd', 'Ningbo Deye Technology Co. Ltd.', 'CHINA GOVERNMENT BOND 3.48% 29.06.2027', 'CHINA GOVERNMENT BOND 4.15% 12.12.2031', 'CHINA GOVERNMENT BOND 2.82% 12.08.2032', 'COUNTRY GARDEN HLDGS 5.125% 14.01.2027', 'COUNTRY GARDEN HLDGS 4.8% 06.08.2030', 'COUNTRY GARDEN HLDGS 3.3% 12.01.2031']</t>
+          <t>['CHINA GOVERNMENT BOND 2.67% 25.05.2033', 'Ping An Bank Co. Ltd.', 'CECEP Solar Energy Co. Ltd.', 'China Vanke Co Ltd', 'China Vanke Co. Ltd.', 'China Baoan Group Co. Ltd.', 'Fuyao Glass Industry Group Co.', 'Pangang Group Vanadium Titaniu', 'Sichuan Chuantou Energy Co. Ltd.', 'Shanghai Baosight Software Co.', 'XCMG Construction Machinery Co.', 'Inner Mongolia Yili Industrial', 'Inner Mongolia Yili Industrial Group Co Ltd', 'Wingtech Technology Co. Ltd.', 'Shanghai Jinjiang Internationa', 'Yutong Bus Co. Ltd.', 'AECC Aero-Engine Control Co. Lt', 'Yunnan Yuntianhua Co. Ltd.', 'Qinghai Salt Lake Industry Co. Ltd.', 'Shanghai International Airport', 'China CSSC Holdings Ltd.', 'Xiamen C &amp; D Inc.', 'Shanghai Construction Group Co.', 'Shanghai Fosun Pharmaceutical', 'Asia - Potash International Investment Guangzhou C', 'Unisplendour Corp. Ltd.', 'Jiangsu Eastern Shenghong Co. L', 'Shanghai International Port Gr', 'Jiangsu Hengrui Pharmaceutical', 'Jiangsu Hengrui Pharmaceuticals Co Ltd', 'Wanhua Chemical Group Co. Ltd.', 'China Avionics Systems Co Ltd A', 'China Merchants Bank Co Ltd', 'China Merchants Bank Co. Ltd.', 'Jiangsu Zhongtian Technology', 'Jiangsu Zhongtian Technology C', 'Jiangsu\xa0Zhongtian\xa0Technology', 'Xiamen Tungsten Co. Ltd.', 'CITIC Securities Co. Ltd.', 'Sichuan Road and Bridge Group', 'Zhangzhou Pientzehuang Pharmac', 'Zhangzhou Pientzehuang Pharmaceutical Co Ltd', 'Sany Heavy Industry Co. Ltd.', 'Zhongjin Gold Corp. Ltd.', 'NARI Technology Co. Ltd.', 'Tongwei Co. Ltd.', 'Zhejiang Sanhua Intelligent Controls Co. Ltd.', 'Bank of China Ltd.', 'Industrial &amp; Commercial Bank o', 'Industrial &amp; Commercial Bank of China Ltd', 'Sinoma Science &amp; Technology Co.', 'Industrial Bank Co. Ltd.', 'TCL Zhonghuan Renewable Energy', 'Bank of Ningbo Co. Ltd.', 'Western Mining Co. Ltd.', 'China Railway Group Ltd.', 'COSCO SHIPPING Development Co.', 'Goldwind Science &amp; Technology', 'Shanghai Electric Group Co. Ltd.', 'China State Construction Engin', 'Aier Eye Hospital Group Co. Ltd.', 'Eve Energy Co. Ltd.', 'Shenzhen Capchem Technology Co.', 'China National Chemical Engine', 'Zhejiang Chint Electrics Co Ltd', 'Zhejiang Chint Electrics Co. Lt', 'East Money Information Co. Ltd.', 'NAURA Technology Group Co. Ltd.', 'JA Solar Technology Co. Ltd.', 'Ganfeng Lithium Group Co Ltd', 'Ganfeng Lithium Group Co. Ltd.', 'Guangzhou Haige Communications', 'Shenzhen Inovance Technology C', 'Shenzhen Inovance Technology Co Ltd', 'Shenzhen Inovance Technology Co., Lt', 'Songcheng Performance Developm', 'Yonghui Superstores Co. Ltd.', 'Tianshan Aluminum Group Co. Ltd.', 'BYD Co Ltd', 'BYD Co. Ltd.', 'Sungrow Power Supply Co Ltd', 'Sungrow Power Supply Co. Ltd.', 'Kuang-Chi Technologies Co. Ltd.', 'Satellite Chemical Co. Ltd.', 'Zhongji Innolight Co. Ltd.', 'LONGi Green Energy Technology', 'Sichuan Hebang Biotechnology C', 'CMOC Group Ltd.', 'Guangzhou Tinci Materials Tech', 'Muyuan Foods Co. Ltd.', 'Foshan Haitian Flavouring &amp; Fo', 'Zhejiang Huayou Cobalt Co. Ltd.', 'Sinomine Resource Group Co. Ltd.', 'Orient Securities Co. Ltd/China', 'China National Nuclear Power C', 'Ningbo Tuopu Group Co. Ltd.', 'Wens Foodstuffs Group Co. Ltd.', 'Yealink Network Technology Cor', 'Foxconn Industrial Internet Co.', 'Contemporary Amperex Technolog', 'Contemporary Amperex Technology Co Ltd', 'Shenzhen Mindray Bio-Medical E', 'Shenzhen Mindray Bio-Medical Electronics Co Ltd', 'Shenzhen Transsion Holdings Co.', 'China Zheshang Bank Co Ltd', 'China Zheshang Bank Co. Ltd.', 'CNGR Advanced Material Co. Ltd.', 'Yunnan Botanee Bio-Technology Group Co. Ltd.', 'China Energy Engineering Corp.', 'China Three Gorges Renewables', 'China Three Gorges Renewables Group Co Ltd', 'Ningbo Deye Technology Co. Ltd.', 'CHINA GOVERNMENT BOND 3.48% 29.06.2027', 'CHINA GOVERNMENT BOND 4.15% 12.12.2031', 'CHINA GOVERNMENT BOND 2.82% 12.08.2032', 'COUNTRY GARDEN HLDGS 5.125% 14.01.2027', 'COUNTRY GARDEN HLDGS 4.8% 06.08.2030', 'COUNTRY GARDEN HLDGS 3.3% 12.01.2031']</t>
         </is>
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>['Kalundborg', 'Fanø', 'Mariagerfjord', 'Odense', 'Randers', 'Esbjerg', 'København', 'Aalborg', 'Aarhus']</t>
+          <t>['Kalundborg', 'Fanø', 'Mariagerfjord', 'Odense', 'Randers', 'København', 'Esbjerg', 'Aalborg', 'Aarhus']</t>
         </is>
       </c>
     </row>
@@ -13152,7 +13152,7 @@
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>['Nigeria, Federal Republic Of (Government) 6.5% 20271128', 'REPUBLIC OF NIGERIA 7.625% 28.11.2047', 'Nigeria, Federal Republic Of (Government) 7.625% 20471128', 'Nigeria, Federal Republic Of (Government) 7.696% 20380223', '7.63% Nigeria Government International Bond 2025', 'Nigeria, Federal Republic Of (Government) 7.625% 20251121', '8.75% Nigeria Government International Bond 2031', 'REPUBLIC OF NIGERIA 8.747% 21.01.2031', 'Nigeria, Federal Republic Of (Government) 8.747% 20310121', 'Nigeria, Federal Republic Of (Government) 9.248% 20490121', 'AFRICA FINANCE CORP 2.875% 28.04.2028', '7,375 NGERIA 28-09-2033 (REGS)', 'REPUBLIC OF NIGERIA 7.375% 28.09.2033', '8,25 NGERIA 28-09-2051 (REGS)', 'REPUBLIC OF NIGERIA 8.25% 28.09.2051', 'Nigeria, Federal Republic Of (Government) 8.25% 20510928', '8.38% Nigeria Government International Bond 2029', '8,375 NGERIA 24-03-2029 (REGS)', 'REPUBLIC OF NIGERIA 8.375% 24.03.2029', 'Nigeria, Federal Republic Of (Government) 8.375% 20290324']</t>
+          <t>['Nigeria, Federal Republic Of (Government) 6.5% 20271128', 'Nigeria, Federal Republic Of (Government) 7.625% 20471128', 'REPUBLIC OF NIGERIA 7.625% 28.11.2047', 'Nigeria, Federal Republic Of (Government) 7.696% 20380223', '7.63% Nigeria Government International Bond 2025', 'Nigeria, Federal Republic Of (Government) 7.625% 20251121', '8.75% Nigeria Government International Bond 2031', 'Nigeria, Federal Republic Of (Government) 8.747% 20310121', 'REPUBLIC OF NIGERIA 8.747% 21.01.2031', 'Nigeria, Federal Republic Of (Government) 9.248% 20490121', 'AFRICA FINANCE CORP 2.875% 28.04.2028', '7,375 NGERIA 28-09-2033 (REGS)', 'REPUBLIC OF NIGERIA 7.375% 28.09.2033', '8,25 NGERIA 28-09-2051 (REGS)', 'Nigeria, Federal Republic Of (Government) 8.25% 20510928', 'REPUBLIC OF NIGERIA 8.25% 28.09.2051', '8,375 NGERIA 24-03-2029 (REGS)', '8.38% Nigeria Government International Bond 2029', 'Nigeria, Federal Republic Of (Government) 8.375% 20290324', 'REPUBLIC OF NIGERIA 8.375% 24.03.2029']</t>
         </is>
       </c>
       <c r="G344" t="inlineStr">
@@ -13184,17 +13184,17 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>['Japan', 'Kikkoman Corp', 'KIKKOMAN CORP', 'Kikkoman Corp.', nan, 'Koito Manufacturing Co. Ltd.', 'Romania Government Bond', 'Rumænien', 'Romania', 'ROMANIA (GOVERNMENT)', 'Romanian Gov.Int. Bond 29.10.2035', 'Romanian Gov.Int. Obligation 29.10.2035', 'Sultanate of Oman', '5.38% Oman Government International Bond 2027', 'Oman Government International Bond', 'Oman', 'OMAN GOV INTERNTL BOND  ', '5.63% Oman Government International Bond 2028', 'Oman Government International Bond 17.01.2048', 'Oman Government International Obligation 17.01.2048', 'ROMANIA  ', 'Romanian Government International Bond', 'Oman Government International Bond 01.02.2025', 'Oman Government International Obligation 01.02.2025', '6.00% Oman Government International Bond 2029', '4.63% Romanian Government International Bond 2049', 'Romanian Government International Bond 03.04.2034', 'Romanian Government International Obligation 03.04.2034', '3.00% Romanian Government International Bond 2031', '4.00% Romanian Government International Bond 2051', '6.75% Oman Government International Bond 2027', 'OMAN SOVEREIGN SUKUK  ', 'Oman Sovereign Sukuk Co', '3.63% Romanian Government International Bond 2032', 'Romanian Government International Bond 25.05.2034', 'Romanian Government International Obligation 25.05.2034', '6.63% Romanian Government International Bond 2028', 'Romania 28', '7.13% Romanian Government International Bond 2033', '5.88% Romanian Government International Bond 2029', '6.38% Romanian Government International Bond 2034']</t>
+          <t>['Kikkoman Corp', 'KIKKOMAN CORP', nan, 'Japan', 'Kikkoman Corp.', 'Koito Manufacturing Co. Ltd.', 'Romania Government Bond', 'Rumænien', 'Romania', 'ROMANIA (GOVERNMENT)', 'Romanian Gov.Int. Bond 29.10.2035', 'Romanian Gov.Int. Obligation 29.10.2035', 'Sultanate of Oman', '5.38% Oman Government International Bond 2027', 'Oman Government International Bond', 'Oman', 'OMAN GOV INTERNTL BOND  ', '5.63% Oman Government International Bond 2028', 'Oman Government International Bond 17.01.2048', 'Oman Government International Obligation 17.01.2048', 'ROMANIA  ', 'Romanian Government International Bond', 'Oman Government International Bond 01.02.2025', 'Oman Government International Obligation 01.02.2025', '6.00% Oman Government International Bond 2029', '4.63% Romanian Government International Bond 2049', 'Romanian Government International Bond 03.04.2034', 'Romanian Government International Obligation 03.04.2034', '3.00% Romanian Government International Bond 2031', '4.00% Romanian Government International Bond 2051', '6.75% Oman Government International Bond 2027', 'OMAN SOVEREIGN SUKUK  ', 'Oman Sovereign Sukuk Co', '3.63% Romanian Government International Bond 2032', 'Romanian Government International Bond 25.05.2034', 'Romanian Government International Obligation 25.05.2034', '6.63% Romanian Government International Bond 2028', 'Romania 28', '7.13% Romanian Government International Bond 2033', '5.88% Romanian Government International Bond 2029', '6.38% Romanian Government International Bond 2034']</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>['Kikkoman Corp.', 'KIKKOMAN CORP', 'Kikkoman Corp', 'Koito Manufacturing Co. Ltd.', '14.02% Cidron Romanov Ltd 2026', 'ROMANIA GOVERNMENT BOND 3.65% 24.09.2031', 'ROMANIA GOVERNMENT BOND 4.85% 25.07.2029', '4,75 ROMGB 11-10-2034 (15Y)', 'ROMANIA GOVERNMENT BOND 2.5% 25.10.2027', '3,25 ROMGB 24-06-2026 (5Y)', 'ROMANIA GOVERNMENT BOND 6.7% 25.02.2032', 'Romania, Republic Of (Government) 6.125% 20440122', 'ROMANI 3 7/8 10/29/35', 'Romanian Government International Bond', '4,75 OMAN 15-06-2026 (REGS)', '5.38% Oman Government International Bond 2027', 'OMAN GOV INTERNTL BOND 6.5% 08.03.2047', '6,5 OMAN 08-03-2047 (REGS)', '5.63% Oman Government International Bond 2028', 'OMAN GOV INTERNTL BOND 6.75% 17.01.2048', 'OMAN 6 3/4 01/17/48', '6,75 OMAN 17-01-2048 (REGS)', 'ROMANIA 3.375% 08.02.2038', 'Romania, Republic Of (Government) 5.125% 20480615', 'OMAN 4 7/8 02/01/25', '6.00% Oman Government International Bond 2029', '6 OMAN 01-08-2029 (REGS)', '4.63% Romanian Government International Bond 2049', 'ROMANI 3 1/2 04/03/34', 'ROMANI 2.124 07/16/31', 'Romania, Republic Of (Government) 2.124% 20310716', 'ROMANI 2 01/28/32', 'Romania, Republic Of (Government) 2% 20320128', 'ROMANIA 3.375% 28.01.2050', 'ROMANI 3.624 05/26/30', 'ROMANIA 3.624% 26.05.2030', '3.00% Romanian Government International Bond 2031', 'Romania, Republic Of (Government) 3% 20310214', '4.00% Romanian Government International Bond 2051', '4 ROMANI 14-02-2051 (REGS)', 'Romania, Republic Of (Government) 4% 20510214', '6.75% Oman Government International Bond 2027', 'OQ SAOC 5.125% 06.05.2028', 'ROMANI 2 5/8 12/02/40', 'ROMANIA 2.625% 02.12.2040', 'Romania, Republic Of (Government) 1.375% 20291202', 'OMAN GOV INTERNTL BOND 7% 25.01.2051', 'BANK MUSCAT SAOG 4.75% 17.03.2026', 'ROMANI 2 04/14/33', 'Romania (Government) 2% 20330414', 'ROMANIA 2.75% 14.04.2041', 'OMAN SOVEREIGN SUKUK 4.875% 15.06.2030', 'Romania (Government) 1.75% 20300713', 'ROMANI 2 7/8 04/13/42', 'ROMANIA 2.875% 13.04.2042', '2,125% Romania 20280307', 'ROMANI 3 3/4 02/07/34', '3.63% Romanian Government International Bond 2032', 'Romania (Government) 3.625% 20320327', 'Romania (Government) 6% 20340525', 'ROMANI 6 05/25/34', '6.63% Romanian Government International Bond 2028', 'Romania 28', '7.13% Romanian Government International Bond 2033', 'Romania (Government) 7.125% 20330117', 'ROMANIA 7.625% 17.01.2053', 'Romania (Government) 7.625% 20530117', 'EDO SUKUK LTD 5.875% 21.09.2033', 'ROMANI 6 3/8 09/18/33', 'ROMANIA 6.375% 18.09.2033', 'ROMANIA 5.5% 18.09.2028', '5.88% Romanian Government International Bond 2029', '5,875 ROMANI 30-01-2029 (REGS)', '6.38% Romanian Government International Bond 2034', 'ROMANI 5 5/8 02/22/36']</t>
+          <t>['KIKKOMAN CORP', 'Kikkoman Corp', 'Kikkoman Corp.', 'Koito Manufacturing Co. Ltd.', '14.02% Cidron Romanov Ltd 2026', 'ROMANIA GOVERNMENT BOND 3.65% 24.09.2031', 'ROMANIA GOVERNMENT BOND 4.85% 25.07.2029', '4,75 ROMGB 11-10-2034 (15Y)', 'ROMANIA GOVERNMENT BOND 2.5% 25.10.2027', '3,25 ROMGB 24-06-2026 (5Y)', 'ROMANIA GOVERNMENT BOND 6.7% 25.02.2032', 'Romania, Republic Of (Government) 6.125% 20440122', 'ROMANI 3 7/8 10/29/35', 'Romanian Government International Bond', '4,75 OMAN 15-06-2026 (REGS)', '5.38% Oman Government International Bond 2027', '6,5 OMAN 08-03-2047 (REGS)', 'OMAN GOV INTERNTL BOND 6.5% 08.03.2047', '5.63% Oman Government International Bond 2028', '6,75 OMAN 17-01-2048 (REGS)', 'OMAN 6 3/4 01/17/48', 'OMAN GOV INTERNTL BOND 6.75% 17.01.2048', 'ROMANIA 3.375% 08.02.2038', 'Romania, Republic Of (Government) 5.125% 20480615', 'OMAN 4 7/8 02/01/25', '6 OMAN 01-08-2029 (REGS)', '6.00% Oman Government International Bond 2029', '4.63% Romanian Government International Bond 2049', 'ROMANI 3 1/2 04/03/34', 'ROMANI 2.124 07/16/31', 'Romania, Republic Of (Government) 2.124% 20310716', 'ROMANI 2 01/28/32', 'Romania, Republic Of (Government) 2% 20320128', 'ROMANIA 3.375% 28.01.2050', 'ROMANI 3.624 05/26/30', 'ROMANIA 3.624% 26.05.2030', '3.00% Romanian Government International Bond 2031', 'Romania, Republic Of (Government) 3% 20310214', '4 ROMANI 14-02-2051 (REGS)', '4.00% Romanian Government International Bond 2051', 'Romania, Republic Of (Government) 4% 20510214', '6.75% Oman Government International Bond 2027', 'OQ SAOC 5.125% 06.05.2028', 'ROMANI 2 5/8 12/02/40', 'ROMANIA 2.625% 02.12.2040', 'Romania, Republic Of (Government) 1.375% 20291202', 'OMAN GOV INTERNTL BOND 7% 25.01.2051', 'BANK MUSCAT SAOG 4.75% 17.03.2026', 'ROMANI 2 04/14/33', 'Romania (Government) 2% 20330414', 'ROMANIA 2.75% 14.04.2041', 'OMAN SOVEREIGN SUKUK 4.875% 15.06.2030', 'Romania (Government) 1.75% 20300713', 'ROMANI 2 7/8 04/13/42', 'ROMANIA 2.875% 13.04.2042', '2,125% Romania 20280307', 'ROMANI 3 3/4 02/07/34', '3.63% Romanian Government International Bond 2032', 'Romania (Government) 3.625% 20320327', 'ROMANI 6 05/25/34', 'Romania (Government) 6% 20340525', '6.63% Romanian Government International Bond 2028', 'Romania 28', '7.13% Romanian Government International Bond 2033', 'Romania (Government) 7.125% 20330117', 'Romania (Government) 7.625% 20530117', 'ROMANIA 7.625% 17.01.2053', 'EDO SUKUK LTD 5.875% 21.09.2033', 'ROMANI 6 3/8 09/18/33', 'ROMANIA 6.375% 18.09.2033', 'ROMANIA 5.5% 18.09.2028', '5,875 ROMANI 30-01-2029 (REGS)', '5.88% Romanian Government International Bond 2029', '6.38% Romanian Government International Bond 2034', 'ROMANI 5 5/8 02/22/36']</t>
         </is>
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>['Fanø', 'Ballerup', 'Brøndby', 'Brønderslev', 'Fredensborg', 'Frederiksberg', 'Furesø', 'Faaborg-Midtfyn', 'Hedensted', 'Herning', 'Hvidovre', 'Ikast-Brande', 'Kerteminde', 'Kolding', 'Køge', 'Lolland', 'Morsø', 'Region Midtjylland', 'Region Nordjylland', 'Region Sjælland', 'Rudersdal', 'Silkeborg', 'Skive', 'Sorø', 'Struer', 'Varde', 'Rødovre', 'Assens', 'Mariagerfjord', 'Odense', 'Aalborg', 'Aarhus', 'Vejen', 'Kalundborg', 'Vesthimmerland', 'Guldborgsund', 'Nordfyn', 'Svendborg', 'Slagelse', 'Greve', 'Fredericia', 'Hillerød', 'Lemvig', 'Aabenraa', 'Ringkøbing-Skjern', 'Vejle']</t>
+          <t>['Ballerup', 'Brøndby', 'Brønderslev', 'Fredensborg', 'Frederiksberg', 'Furesø', 'Faaborg-Midtfyn', 'Hedensted', 'Herning', 'Hvidovre', 'Ikast-Brande', 'Kerteminde', 'Kolding', 'Køge', 'Lolland', 'Morsø', 'Region Midtjylland', 'Region Nordjylland', 'Region Sjælland', 'Rudersdal', 'Silkeborg', 'Skive', 'Sorø', 'Struer', 'Varde', 'Assens', 'Mariagerfjord', 'Odense', 'Aalborg', 'Fanø', 'Rødovre', 'Aarhus', 'Vejen', 'Kalundborg', 'Vesthimmerland', 'Guldborgsund', 'Nordfyn', 'Greve', 'Fredericia', 'Hillerød', 'Lemvig', 'Aabenraa', 'Svendborg', 'Slagelse', 'Ringkøbing-Skjern', 'Vejle']</t>
         </is>
       </c>
     </row>
@@ -13226,7 +13226,7 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>['8.25% Pakistan Government International Bond 2024', 'ISLAMIC REP OF PAKISTAN 6.875% 05.12.2027', 'ISLAMIC REP OF PAKISTAN 6% 08.04.2026', 'ISLAMIC REP OF PAKISTAN 7.375% 08.04.2031', 'ISLAMIC REP OF PAKISTAN 8.875% 08.04.2051', '8,875 PKSTAN 08-04-2051 (REGS)', 'PAKISTAN WATER &amp; POWER 7.5% 04.06.2031', '7,95 PKSTAN 31-01-2029 (REGS)']</t>
+          <t>['8.25% Pakistan Government International Bond 2024', 'ISLAMIC REP OF PAKISTAN 6.875% 05.12.2027', 'ISLAMIC REP OF PAKISTAN 6% 08.04.2026', 'ISLAMIC REP OF PAKISTAN 7.375% 08.04.2031', '8,875 PKSTAN 08-04-2051 (REGS)', 'ISLAMIC REP OF PAKISTAN 8.875% 08.04.2051', 'PAKISTAN WATER &amp; POWER 7.5% 04.06.2031', '7,95 PKSTAN 31-01-2029 (REGS)']</t>
         </is>
       </c>
       <c r="G346" t="inlineStr">
@@ -13258,17 +13258,17 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>['Qatar', nan, 'Qatar National Bank QPSC', 'State of Qatar', '5.10% Qatar Government International Bond 2048', 'Qatar Government International Bond', 'STATE OF QATAR  ', 'QATAR ENERGY  ', 'QatarEnergy']</t>
+          <t>['Qatar', nan, 'Qatar National Bank QPSC', 'State of Qatar', '5.10% Qatar Government International Bond 2048', 'Qatar Government International Bond', 'STATE OF QATAR  ', 'QatarEnergy', 'QATAR ENERGY  ']</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>['Qatar Islamic Bank SAQ', 'Qatar National Bank QPSC', 'Ooredoo QPSC', 'Commercial Bank PSQC/The', 'Industries Qatar QSC', 'Masraf Al Rayan QSC', '3,25 QATAR 02-06-2026 (REGS)', '4,5 QATAR 23-04-2028 (REGS)', '5.10% Qatar Government International Bond 2048', 'STATE OF QATAR 5.103% 23.04.2048', 'STATE OF QATAR 4.817% 14.03.2049', 'STATE OF QATAR 3.4% 16.04.2025', '3,75 QATAR 16-04-2030 (REGS)', 'STATE OF QATAR 4.4% 16.04.2050', '4,4 QATAR 16-04-2050 (REGS)', 'QATAR ENERGY 2.25% 12.07.2031', '2,25 QPETRO 12-07-2031 (REGS)']</t>
+          <t>['Qatar Islamic Bank SAQ', 'Qatar National Bank QPSC', 'Ooredoo QPSC', 'Commercial Bank PSQC/The', 'Industries Qatar QSC', 'Masraf Al Rayan QSC', '3,25 QATAR 02-06-2026 (REGS)', '4,5 QATAR 23-04-2028 (REGS)', '5.10% Qatar Government International Bond 2048', 'STATE OF QATAR 5.103% 23.04.2048', 'STATE OF QATAR 4.817% 14.03.2049', 'STATE OF QATAR 3.4% 16.04.2025', '3,75 QATAR 16-04-2030 (REGS)', '4,4 QATAR 16-04-2050 (REGS)', 'STATE OF QATAR 4.4% 16.04.2050', '2,25 QPETRO 12-07-2031 (REGS)', 'QATAR ENERGY 2.25% 12.07.2031']</t>
         </is>
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>['Fanø', 'Mariagerfjord', 'Rudersdal', 'Herning', 'Ringkøbing-Skjern', 'Kalundborg', 'Region Nordjylland', 'Rødovre', 'Vejen']</t>
+          <t>['Fanø', 'Mariagerfjord', 'Rudersdal', 'Herning', 'Ringkøbing-Skjern', 'Region Nordjylland', 'Kalundborg', 'Rødovre', 'Vejen']</t>
         </is>
       </c>
     </row>
@@ -13295,17 +13295,17 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>['5.50% Rwanda International Government Bond 2031', 'Republic of Rwanda', 'REPUBLIC OF RWANDA  ', 'Rwanda', 'Rwanda International Government Bond']</t>
+          <t>['Republic of Rwanda', '5.50% Rwanda International Government Bond 2031', 'Rwanda International Government Bond', 'REPUBLIC OF RWANDA  ', 'Rwanda']</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>['5.50% Rwanda International Government Bond 2031', '5,5 RWANDA 09-08-2031 (REGS)', 'REPUBLIC OF RWANDA 5.5% 09.08.2031']</t>
+          <t>['5,5 RWANDA 09-08-2031 (REGS)', '5.50% Rwanda International Government Bond 2031', 'REPUBLIC OF RWANDA 5.5% 09.08.2031']</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>['Ringkøbing-Skjern', 'Herning', 'Kalundborg', 'Fanø', 'Region Nordjylland', 'Rødovre', 'Vejen']</t>
+          <t>['Herning', 'Ringkøbing-Skjern', 'Region Nordjylland', 'Kalundborg', 'Fanø', 'Rødovre', 'Vejen']</t>
         </is>
       </c>
     </row>
@@ -13443,17 +13443,17 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>[nan, '5.38% Republic of Uzbekistan International Bond 2029', 'Republic of Uzbekistan', 'REPUBLIC OF UZBEKISTAN  ', 'Republic of Uzbekistan International Bond', 'Uzbekistan', 'National Bank of Uzbekistan', '3.70% Republic of Uzbekistan International Bond 2030', '7.85% Republic of Uzbekistan International Bond 2028', 'UZBEKISTAN INTL BOND  ']</t>
+          <t>['Republic of Uzbekistan', '5.38% Republic of Uzbekistan International Bond 2029', 'REPUBLIC OF UZBEKISTAN  ', 'Republic of Uzbekistan International Bond', 'Uzbekistan', nan, 'National Bank of Uzbekistan', '3.70% Republic of Uzbekistan International Bond 2030', '7.85% Republic of Uzbekistan International Bond 2028', 'UZBEKISTAN INTL BOND  ']</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>['Republic of Uzbekistan International Bond', '5.38% Republic of Uzbekistan International Bond 2029', '5,375 UZBEK 20-02-2029 (REGS)', 'REPUBLIC OF UZBEKISTAN 5.375% 20.02.2029', '4,75 UNGUZB 16-11-2028 (REGS)', 'UZBEKNEFTEGAZ JSC 4.75% 16.11.2028', 'NATIONAL BANK OF UZBEKIS 4.85% 21.10.2025', 'IPOTEKA-BANK ATIB 5.5% 19.11.2025', '3.70% Republic of Uzbekistan International Bond 2030', 'REPUBLIC OF UZBEKISTAN 3.7% 25.11.2030', '3.90% Republic of Uzbekistan International Bond 2031', '7.85% Republic of Uzbekistan International Bond 2028', '6,9 UZBEK 28-02-2032 (REGS)', '6.90% Republic of Uzbekistan International Bond 2032', 'UZBEKISTAN INTL BOND 6.9% 28.02.2032', '5.38% Republic of Uzbekistan International Bond 2027', 'UZBEKISTAN INTL BOND 5.375% 29.05.2027', 'NATIONAL BANK OF UZBEKIS 8.5% 05.07.2029']</t>
+          <t>['5,375 UZBEK 20-02-2029 (REGS)', '5.38% Republic of Uzbekistan International Bond 2029', 'REPUBLIC OF UZBEKISTAN 5.375% 20.02.2029', 'Republic of Uzbekistan International Bond', '4,75 UNGUZB 16-11-2028 (REGS)', 'UZBEKNEFTEGAZ JSC 4.75% 16.11.2028', 'NATIONAL BANK OF UZBEKIS 4.85% 21.10.2025', 'IPOTEKA-BANK ATIB 5.5% 19.11.2025', '3.70% Republic of Uzbekistan International Bond 2030', 'REPUBLIC OF UZBEKISTAN 3.7% 25.11.2030', '3.90% Republic of Uzbekistan International Bond 2031', '7.85% Republic of Uzbekistan International Bond 2028', '6,9 UZBEK 28-02-2032 (REGS)', '6.90% Republic of Uzbekistan International Bond 2032', 'UZBEKISTAN INTL BOND 6.9% 28.02.2032', '5.38% Republic of Uzbekistan International Bond 2027', 'UZBEKISTAN INTL BOND 5.375% 29.05.2027', 'NATIONAL BANK OF UZBEKIS 8.5% 05.07.2029']</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>['Svendborg', 'Ringkøbing-Skjern', 'Hedensted', 'Slagelse', 'Herning', 'Kalundborg', 'Rødovre', 'Vejen', 'Fanø', 'Region Nordjylland']</t>
+          <t>['Herning', 'Ringkøbing-Skjern', 'Kalundborg', 'Rødovre', 'Vejen', 'Fanø', 'Svendborg', 'Hedensted', 'Slagelse', 'Region Nordjylland']</t>
         </is>
       </c>
     </row>

</xml_diff>